<commit_message>
adicionando colunas para a visualização
</commit_message>
<xml_diff>
--- a/dicionario-ed-superior-inep.xlsx
+++ b/dicionario-ed-superior-inep.xlsx
@@ -2524,14 +2524,38 @@
     <xf numFmtId="0" fontId="17" fillId="8" borderId="5" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2550,18 +2574,6 @@
     </xf>
     <xf numFmtId="49" fontId="8" fillId="5" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2587,18 +2599,6 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2621,6 +2621,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2824,10 +2828,10 @@
   <dimension ref="A1:Z91"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="8" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="8" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2934,29 +2938,29 @@
       <c r="Z3" s="2"/>
     </row>
     <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="98" t="s">
         <v>524</v>
       </c>
-      <c r="B4" s="104"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="104"/>
-      <c r="N4" s="104"/>
-      <c r="O4" s="104"/>
-      <c r="P4" s="104"/>
-      <c r="Q4" s="104"/>
-      <c r="R4" s="104"/>
-      <c r="S4" s="104"/>
-      <c r="T4" s="105"/>
-      <c r="U4" s="104"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="99"/>
+      <c r="N4" s="99"/>
+      <c r="O4" s="99"/>
+      <c r="P4" s="99"/>
+      <c r="Q4" s="99"/>
+      <c r="R4" s="99"/>
+      <c r="S4" s="99"/>
+      <c r="T4" s="100"/>
+      <c r="U4" s="99"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
@@ -2992,43 +2996,43 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="96" t="s">
+      <c r="A6" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="96" t="s">
+      <c r="C6" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="96" t="s">
+      <c r="D6" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="96" t="s">
+      <c r="E6" s="101" t="s">
         <v>185</v>
       </c>
-      <c r="F6" s="96" t="s">
+      <c r="F6" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="96" t="s">
+      <c r="G6" s="101" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="100" t="s">
+      <c r="H6" s="108" t="s">
         <v>176</v>
       </c>
-      <c r="I6" s="101"/>
-      <c r="J6" s="101"/>
-      <c r="K6" s="101"/>
-      <c r="L6" s="101"/>
-      <c r="M6" s="101"/>
-      <c r="N6" s="101"/>
-      <c r="O6" s="101"/>
-      <c r="P6" s="101"/>
-      <c r="Q6" s="101"/>
-      <c r="R6" s="101"/>
-      <c r="S6" s="101"/>
-      <c r="T6" s="102"/>
-      <c r="U6" s="98" t="s">
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="109"/>
+      <c r="M6" s="109"/>
+      <c r="N6" s="109"/>
+      <c r="O6" s="109"/>
+      <c r="P6" s="109"/>
+      <c r="Q6" s="109"/>
+      <c r="R6" s="109"/>
+      <c r="S6" s="109"/>
+      <c r="T6" s="110"/>
+      <c r="U6" s="106" t="s">
         <v>7</v>
       </c>
       <c r="V6" s="2"/>
@@ -3038,13 +3042,13 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="106"/>
-      <c r="B7" s="106"/>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="97"/>
-      <c r="G7" s="106"/>
+      <c r="A7" s="102"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="102"/>
       <c r="H7" s="6" t="s">
         <v>8</v>
       </c>
@@ -3084,7 +3088,7 @@
       <c r="T7" s="6" t="s">
         <v>614</v>
       </c>
-      <c r="U7" s="99"/>
+      <c r="U7" s="107"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
@@ -3184,29 +3188,29 @@
       <c r="Z9" s="7"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="95"/>
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="95"/>
-      <c r="I10" s="95"/>
-      <c r="J10" s="95"/>
-      <c r="K10" s="95"/>
-      <c r="L10" s="95"/>
-      <c r="M10" s="95"/>
-      <c r="N10" s="95"/>
-      <c r="O10" s="95"/>
-      <c r="P10" s="95"/>
-      <c r="Q10" s="95"/>
-      <c r="R10" s="95"/>
-      <c r="S10" s="95"/>
-      <c r="T10" s="95"/>
-      <c r="U10" s="95"/>
+      <c r="B10" s="104"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="104"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="104"/>
+      <c r="L10" s="104"/>
+      <c r="M10" s="104"/>
+      <c r="N10" s="104"/>
+      <c r="O10" s="104"/>
+      <c r="P10" s="104"/>
+      <c r="Q10" s="104"/>
+      <c r="R10" s="104"/>
+      <c r="S10" s="104"/>
+      <c r="T10" s="104"/>
+      <c r="U10" s="104"/>
       <c r="V10" s="8"/>
       <c r="W10" s="8"/>
       <c r="X10" s="8"/>
@@ -3281,7 +3285,7 @@
       <c r="A12" s="31">
         <v>3</v>
       </c>
-      <c r="B12" s="118" t="s">
+      <c r="B12" s="97" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="34" t="s">
@@ -3473,7 +3477,7 @@
       <c r="A15" s="31">
         <v>6</v>
       </c>
-      <c r="B15" s="118" t="s">
+      <c r="B15" s="97" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="30" t="s">
@@ -3601,7 +3605,7 @@
       <c r="A17" s="31">
         <v>8</v>
       </c>
-      <c r="B17" s="118" t="s">
+      <c r="B17" s="97" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="30" t="s">
@@ -3728,10 +3732,10 @@
       <c r="Z18" s="9"/>
     </row>
     <row r="19" spans="1:26" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="116">
+      <c r="A19" s="95">
         <v>10</v>
       </c>
-      <c r="B19" s="117" t="s">
+      <c r="B19" s="96" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="32" t="s">
@@ -3792,10 +3796,10 @@
       <c r="Z19" s="9"/>
     </row>
     <row r="20" spans="1:26" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="116">
+      <c r="A20" s="95">
         <v>11</v>
       </c>
-      <c r="B20" s="118" t="s">
+      <c r="B20" s="97" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="34" t="s">
@@ -3856,10 +3860,10 @@
       <c r="Z20" s="9"/>
     </row>
     <row r="21" spans="1:26" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="116">
+      <c r="A21" s="95">
         <v>12</v>
       </c>
-      <c r="B21" s="117" t="s">
+      <c r="B21" s="96" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="32" t="s">
@@ -3920,10 +3924,10 @@
       <c r="Z21" s="9"/>
     </row>
     <row r="22" spans="1:26" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="116">
+      <c r="A22" s="95">
         <v>13</v>
       </c>
-      <c r="B22" s="118" t="s">
+      <c r="B22" s="97" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="34" t="s">
@@ -4120,10 +4124,10 @@
       <c r="Z24" s="9"/>
     </row>
     <row r="25" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="116">
+      <c r="A25" s="95">
         <v>16</v>
       </c>
-      <c r="B25" s="118" t="s">
+      <c r="B25" s="97" t="s">
         <v>59</v>
       </c>
       <c r="C25" s="30" t="s">
@@ -4184,10 +4188,10 @@
       <c r="Z25" s="15"/>
     </row>
     <row r="26" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="116">
+      <c r="A26" s="95">
         <v>17</v>
       </c>
-      <c r="B26" s="118" t="s">
+      <c r="B26" s="97" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="14" t="s">
@@ -4248,10 +4252,10 @@
       <c r="Z26" s="15"/>
     </row>
     <row r="27" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="116">
+      <c r="A27" s="95">
         <v>18</v>
       </c>
-      <c r="B27" s="117" t="s">
+      <c r="B27" s="96" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="36" t="s">
@@ -4312,10 +4316,10 @@
       <c r="Z27" s="9"/>
     </row>
     <row r="28" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="116">
+      <c r="A28" s="95">
         <v>19</v>
       </c>
-      <c r="B28" s="117" t="s">
+      <c r="B28" s="96" t="s">
         <v>49</v>
       </c>
       <c r="C28" s="36" t="s">
@@ -4376,10 +4380,10 @@
       <c r="Z28" s="9"/>
     </row>
     <row r="29" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="116">
+      <c r="A29" s="95">
         <v>20</v>
       </c>
-      <c r="B29" s="117" t="s">
+      <c r="B29" s="96" t="s">
         <v>109</v>
       </c>
       <c r="C29" s="36" t="s">
@@ -4440,10 +4444,10 @@
       <c r="Z29" s="9"/>
     </row>
     <row r="30" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="116">
-        <v>21</v>
-      </c>
-      <c r="B30" s="117" t="s">
+      <c r="A30" s="95">
+        <v>21</v>
+      </c>
+      <c r="B30" s="96" t="s">
         <v>50</v>
       </c>
       <c r="C30" s="36" t="s">
@@ -4504,10 +4508,10 @@
       <c r="Z30" s="9"/>
     </row>
     <row r="31" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="116">
-        <v>22</v>
-      </c>
-      <c r="B31" s="117" t="s">
+      <c r="A31" s="95">
+        <v>22</v>
+      </c>
+      <c r="B31" s="96" t="s">
         <v>51</v>
       </c>
       <c r="C31" s="32" t="s">
@@ -4568,10 +4572,10 @@
       <c r="Z31" s="9"/>
     </row>
     <row r="32" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="116">
+      <c r="A32" s="95">
         <v>23</v>
       </c>
-      <c r="B32" s="117" t="s">
+      <c r="B32" s="96" t="s">
         <v>52</v>
       </c>
       <c r="C32" s="32" t="s">
@@ -4632,10 +4636,10 @@
       <c r="Z32" s="9"/>
     </row>
     <row r="33" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="116">
+      <c r="A33" s="95">
         <v>24</v>
       </c>
-      <c r="B33" s="117" t="s">
+      <c r="B33" s="96" t="s">
         <v>53</v>
       </c>
       <c r="C33" s="36" t="s">
@@ -4696,10 +4700,10 @@
       <c r="Z33" s="9"/>
     </row>
     <row r="34" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="116">
+      <c r="A34" s="95">
         <v>25</v>
       </c>
-      <c r="B34" s="117" t="s">
+      <c r="B34" s="96" t="s">
         <v>54</v>
       </c>
       <c r="C34" s="36" t="s">
@@ -4760,10 +4764,10 @@
       <c r="Z34" s="9"/>
     </row>
     <row r="35" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A35" s="116">
+      <c r="A35" s="95">
         <v>26</v>
       </c>
-      <c r="B35" s="117" t="s">
+      <c r="B35" s="96" t="s">
         <v>65</v>
       </c>
       <c r="C35" s="36" t="s">
@@ -4824,10 +4828,10 @@
       <c r="Z35" s="15"/>
     </row>
     <row r="36" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A36" s="116">
+      <c r="A36" s="95">
         <v>27</v>
       </c>
-      <c r="B36" s="117" t="s">
+      <c r="B36" s="96" t="s">
         <v>67</v>
       </c>
       <c r="C36" s="36" t="s">
@@ -4888,10 +4892,10 @@
       <c r="Z36" s="15"/>
     </row>
     <row r="37" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A37" s="116">
+      <c r="A37" s="95">
         <v>28</v>
       </c>
-      <c r="B37" s="117" t="s">
+      <c r="B37" s="96" t="s">
         <v>69</v>
       </c>
       <c r="C37" s="36" t="s">
@@ -4952,10 +4956,10 @@
       <c r="Z37" s="15"/>
     </row>
     <row r="38" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A38" s="116">
+      <c r="A38" s="95">
         <v>29</v>
       </c>
-      <c r="B38" s="117" t="s">
+      <c r="B38" s="96" t="s">
         <v>71</v>
       </c>
       <c r="C38" s="36" t="s">
@@ -5016,10 +5020,10 @@
       <c r="Z38" s="15"/>
     </row>
     <row r="39" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A39" s="116">
+      <c r="A39" s="95">
         <v>30</v>
       </c>
-      <c r="B39" s="117" t="s">
+      <c r="B39" s="96" t="s">
         <v>73</v>
       </c>
       <c r="C39" s="36" t="s">
@@ -5080,10 +5084,10 @@
       <c r="Z39" s="15"/>
     </row>
     <row r="40" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A40" s="116">
+      <c r="A40" s="95">
         <v>31</v>
       </c>
-      <c r="B40" s="117" t="s">
+      <c r="B40" s="96" t="s">
         <v>75</v>
       </c>
       <c r="C40" s="36" t="s">
@@ -5144,10 +5148,10 @@
       <c r="Z40" s="15"/>
     </row>
     <row r="41" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A41" s="116">
+      <c r="A41" s="95">
         <v>32</v>
       </c>
-      <c r="B41" s="117" t="s">
+      <c r="B41" s="96" t="s">
         <v>77</v>
       </c>
       <c r="C41" s="36" t="s">
@@ -5208,10 +5212,10 @@
       <c r="Z41" s="15"/>
     </row>
     <row r="42" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A42" s="116">
+      <c r="A42" s="95">
         <v>33</v>
       </c>
-      <c r="B42" s="117" t="s">
+      <c r="B42" s="96" t="s">
         <v>79</v>
       </c>
       <c r="C42" s="36" t="s">
@@ -5272,10 +5276,10 @@
       <c r="Z42" s="15"/>
     </row>
     <row r="43" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A43" s="116">
+      <c r="A43" s="95">
         <v>34</v>
       </c>
-      <c r="B43" s="117" t="s">
+      <c r="B43" s="96" t="s">
         <v>81</v>
       </c>
       <c r="C43" s="36" t="s">
@@ -5336,10 +5340,10 @@
       <c r="Z43" s="15"/>
     </row>
     <row r="44" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A44" s="116">
+      <c r="A44" s="95">
         <v>35</v>
       </c>
-      <c r="B44" s="117" t="s">
+      <c r="B44" s="96" t="s">
         <v>83</v>
       </c>
       <c r="C44" s="36" t="s">
@@ -5400,10 +5404,10 @@
       <c r="Z44" s="15"/>
     </row>
     <row r="45" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A45" s="116">
+      <c r="A45" s="95">
         <v>36</v>
       </c>
-      <c r="B45" s="117" t="s">
+      <c r="B45" s="96" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="36" t="s">
@@ -5464,10 +5468,10 @@
       <c r="Z45" s="15"/>
     </row>
     <row r="46" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A46" s="116">
+      <c r="A46" s="95">
         <v>37</v>
       </c>
-      <c r="B46" s="117" t="s">
+      <c r="B46" s="96" t="s">
         <v>87</v>
       </c>
       <c r="C46" s="36" t="s">
@@ -5528,10 +5532,10 @@
       <c r="Z46" s="15"/>
     </row>
     <row r="47" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A47" s="116">
+      <c r="A47" s="95">
         <v>38</v>
       </c>
-      <c r="B47" s="117" t="s">
+      <c r="B47" s="96" t="s">
         <v>89</v>
       </c>
       <c r="C47" s="36" t="s">
@@ -5592,10 +5596,10 @@
       <c r="Z47" s="15"/>
     </row>
     <row r="48" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A48" s="116">
+      <c r="A48" s="95">
         <v>39</v>
       </c>
-      <c r="B48" s="117" t="s">
+      <c r="B48" s="96" t="s">
         <v>91</v>
       </c>
       <c r="C48" s="36" t="s">
@@ -5656,10 +5660,10 @@
       <c r="Z48" s="15"/>
     </row>
     <row r="49" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A49" s="116">
+      <c r="A49" s="95">
         <v>40</v>
       </c>
-      <c r="B49" s="117" t="s">
+      <c r="B49" s="96" t="s">
         <v>93</v>
       </c>
       <c r="C49" s="36" t="s">
@@ -5720,10 +5724,10 @@
       <c r="Z49" s="15"/>
     </row>
     <row r="50" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A50" s="116">
+      <c r="A50" s="95">
         <v>41</v>
       </c>
-      <c r="B50" s="117" t="s">
+      <c r="B50" s="96" t="s">
         <v>95</v>
       </c>
       <c r="C50" s="32" t="s">
@@ -5786,10 +5790,10 @@
       <c r="Z50" s="15"/>
     </row>
     <row r="51" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A51" s="116">
+      <c r="A51" s="95">
         <v>42</v>
       </c>
-      <c r="B51" s="117" t="s">
+      <c r="B51" s="96" t="s">
         <v>96</v>
       </c>
       <c r="C51" s="32" t="s">
@@ -5854,10 +5858,10 @@
       <c r="Z51" s="15"/>
     </row>
     <row r="52" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A52" s="116">
+      <c r="A52" s="95">
         <v>43</v>
       </c>
-      <c r="B52" s="117" t="s">
+      <c r="B52" s="96" t="s">
         <v>98</v>
       </c>
       <c r="C52" s="32" t="s">
@@ -5922,10 +5926,10 @@
       <c r="Z52" s="15"/>
     </row>
     <row r="53" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A53" s="116">
+      <c r="A53" s="95">
         <v>44</v>
       </c>
-      <c r="B53" s="117" t="s">
+      <c r="B53" s="96" t="s">
         <v>100</v>
       </c>
       <c r="C53" s="36" t="s">
@@ -5990,10 +5994,10 @@
       <c r="Z53" s="15"/>
     </row>
     <row r="54" spans="1:26" ht="34.200000000000003" x14ac:dyDescent="0.25">
-      <c r="A54" s="116">
+      <c r="A54" s="95">
         <v>45</v>
       </c>
-      <c r="B54" s="117" t="s">
+      <c r="B54" s="96" t="s">
         <v>102</v>
       </c>
       <c r="C54" s="32" t="s">
@@ -6058,10 +6062,10 @@
       <c r="Z54" s="15"/>
     </row>
     <row r="55" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A55" s="116">
+      <c r="A55" s="95">
         <v>46</v>
       </c>
-      <c r="B55" s="117" t="s">
+      <c r="B55" s="96" t="s">
         <v>104</v>
       </c>
       <c r="C55" s="36" t="s">
@@ -6126,10 +6130,10 @@
       <c r="Z55" s="15"/>
     </row>
     <row r="56" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A56" s="116">
+      <c r="A56" s="95">
         <v>47</v>
       </c>
-      <c r="B56" s="117" t="s">
+      <c r="B56" s="96" t="s">
         <v>105</v>
       </c>
       <c r="C56" s="32" t="s">
@@ -6194,10 +6198,10 @@
       <c r="Z56" s="15"/>
     </row>
     <row r="57" spans="1:26" ht="34.200000000000003" x14ac:dyDescent="0.25">
-      <c r="A57" s="116">
+      <c r="A57" s="95">
         <v>48</v>
       </c>
-      <c r="B57" s="117" t="s">
+      <c r="B57" s="96" t="s">
         <v>106</v>
       </c>
       <c r="C57" s="32" t="s">
@@ -6262,10 +6266,10 @@
       <c r="Z57" s="15"/>
     </row>
     <row r="58" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A58" s="116">
+      <c r="A58" s="95">
         <v>49</v>
       </c>
-      <c r="B58" s="117" t="s">
+      <c r="B58" s="96" t="s">
         <v>107</v>
       </c>
       <c r="C58" s="36" t="s">
@@ -6328,10 +6332,10 @@
       <c r="Z58" s="15"/>
     </row>
     <row r="59" spans="1:26" ht="34.200000000000003" x14ac:dyDescent="0.25">
-      <c r="A59" s="116">
+      <c r="A59" s="95">
         <v>50</v>
       </c>
-      <c r="B59" s="117" t="s">
+      <c r="B59" s="96" t="s">
         <v>108</v>
       </c>
       <c r="C59" s="32" t="s">
@@ -6394,29 +6398,29 @@
       <c r="Z59" s="15"/>
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="94" t="s">
+      <c r="A60" s="103" t="s">
         <v>111</v>
       </c>
-      <c r="B60" s="95"/>
-      <c r="C60" s="95"/>
-      <c r="D60" s="95"/>
-      <c r="E60" s="95"/>
-      <c r="F60" s="95"/>
-      <c r="G60" s="95"/>
-      <c r="H60" s="95"/>
-      <c r="I60" s="95"/>
-      <c r="J60" s="95"/>
-      <c r="K60" s="95"/>
-      <c r="L60" s="95"/>
-      <c r="M60" s="95"/>
-      <c r="N60" s="95"/>
-      <c r="O60" s="95"/>
-      <c r="P60" s="95"/>
-      <c r="Q60" s="95"/>
-      <c r="R60" s="95"/>
-      <c r="S60" s="95"/>
-      <c r="T60" s="95"/>
-      <c r="U60" s="95"/>
+      <c r="B60" s="104"/>
+      <c r="C60" s="104"/>
+      <c r="D60" s="104"/>
+      <c r="E60" s="104"/>
+      <c r="F60" s="104"/>
+      <c r="G60" s="104"/>
+      <c r="H60" s="104"/>
+      <c r="I60" s="104"/>
+      <c r="J60" s="104"/>
+      <c r="K60" s="104"/>
+      <c r="L60" s="104"/>
+      <c r="M60" s="104"/>
+      <c r="N60" s="104"/>
+      <c r="O60" s="104"/>
+      <c r="P60" s="104"/>
+      <c r="Q60" s="104"/>
+      <c r="R60" s="104"/>
+      <c r="S60" s="104"/>
+      <c r="T60" s="104"/>
+      <c r="U60" s="104"/>
       <c r="V60" s="8"/>
       <c r="W60" s="8"/>
       <c r="X60" s="8"/>
@@ -7000,10 +7004,10 @@
       <c r="Z69" s="15"/>
     </row>
     <row r="70" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A70" s="116">
+      <c r="A70" s="95">
         <v>60</v>
       </c>
-      <c r="B70" s="117" t="s">
+      <c r="B70" s="96" t="s">
         <v>406</v>
       </c>
       <c r="C70" s="32" t="s">
@@ -7064,10 +7068,10 @@
       <c r="Z70" s="15"/>
     </row>
     <row r="71" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A71" s="116">
+      <c r="A71" s="95">
         <v>61</v>
       </c>
-      <c r="B71" s="117" t="s">
+      <c r="B71" s="96" t="s">
         <v>407</v>
       </c>
       <c r="C71" s="32" t="s">
@@ -7128,10 +7132,10 @@
       <c r="Z71" s="15"/>
     </row>
     <row r="72" spans="1:26" ht="22.8" x14ac:dyDescent="0.25">
-      <c r="A72" s="116">
+      <c r="A72" s="95">
         <v>62</v>
       </c>
-      <c r="B72" s="117" t="s">
+      <c r="B72" s="96" t="s">
         <v>408</v>
       </c>
       <c r="C72" s="32" t="s">
@@ -7192,10 +7196,10 @@
       <c r="Z72" s="15"/>
     </row>
     <row r="73" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A73" s="116">
+      <c r="A73" s="95">
         <v>63</v>
       </c>
-      <c r="B73" s="117" t="s">
+      <c r="B73" s="96" t="s">
         <v>409</v>
       </c>
       <c r="C73" s="32" t="s">
@@ -7256,10 +7260,10 @@
       <c r="Z73" s="15"/>
     </row>
     <row r="74" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A74" s="116">
+      <c r="A74" s="95">
         <v>64</v>
       </c>
-      <c r="B74" s="117" t="s">
+      <c r="B74" s="96" t="s">
         <v>410</v>
       </c>
       <c r="C74" s="32" t="s">
@@ -7320,10 +7324,10 @@
       <c r="Z74" s="15"/>
     </row>
     <row r="75" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A75" s="116">
+      <c r="A75" s="95">
         <v>65</v>
       </c>
-      <c r="B75" s="117" t="s">
+      <c r="B75" s="96" t="s">
         <v>411</v>
       </c>
       <c r="C75" s="32" t="s">
@@ -7384,10 +7388,10 @@
       <c r="Z75" s="15"/>
     </row>
     <row r="76" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A76" s="116">
+      <c r="A76" s="95">
         <v>66</v>
       </c>
-      <c r="B76" s="117" t="s">
+      <c r="B76" s="96" t="s">
         <v>412</v>
       </c>
       <c r="C76" s="32" t="s">
@@ -7448,10 +7452,10 @@
       <c r="Z76" s="15"/>
     </row>
     <row r="77" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A77" s="116">
+      <c r="A77" s="95">
         <v>67</v>
       </c>
-      <c r="B77" s="117" t="s">
+      <c r="B77" s="96" t="s">
         <v>413</v>
       </c>
       <c r="C77" s="32" t="s">
@@ -7512,10 +7516,10 @@
       <c r="Z77" s="15"/>
     </row>
     <row r="78" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A78" s="116">
+      <c r="A78" s="95">
         <v>68</v>
       </c>
-      <c r="B78" s="117" t="s">
+      <c r="B78" s="96" t="s">
         <v>414</v>
       </c>
       <c r="C78" s="32" t="s">
@@ -7576,10 +7580,10 @@
       <c r="Z78" s="15"/>
     </row>
     <row r="79" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A79" s="116">
+      <c r="A79" s="95">
         <v>69</v>
       </c>
-      <c r="B79" s="117" t="s">
+      <c r="B79" s="96" t="s">
         <v>415</v>
       </c>
       <c r="C79" s="32" t="s">
@@ -7640,10 +7644,10 @@
       <c r="Z79" s="15"/>
     </row>
     <row r="80" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A80" s="116">
+      <c r="A80" s="95">
         <v>70</v>
       </c>
-      <c r="B80" s="117" t="s">
+      <c r="B80" s="96" t="s">
         <v>416</v>
       </c>
       <c r="C80" s="32" t="s">
@@ -7704,10 +7708,10 @@
       <c r="Z80" s="15"/>
     </row>
     <row r="81" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A81" s="116">
+      <c r="A81" s="95">
         <v>71</v>
       </c>
-      <c r="B81" s="117" t="s">
+      <c r="B81" s="96" t="s">
         <v>417</v>
       </c>
       <c r="C81" s="32" t="s">
@@ -7768,10 +7772,10 @@
       <c r="Z81" s="15"/>
     </row>
     <row r="82" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A82" s="116">
+      <c r="A82" s="95">
         <v>72</v>
       </c>
-      <c r="B82" s="117" t="s">
+      <c r="B82" s="96" t="s">
         <v>418</v>
       </c>
       <c r="C82" s="32" t="s">
@@ -7832,10 +7836,10 @@
       <c r="Z82" s="15"/>
     </row>
     <row r="83" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A83" s="116">
+      <c r="A83" s="95">
         <v>73</v>
       </c>
-      <c r="B83" s="115" t="s">
+      <c r="B83" s="94" t="s">
         <v>419</v>
       </c>
       <c r="C83" s="32" t="s">
@@ -7896,10 +7900,10 @@
       <c r="Z83" s="15"/>
     </row>
     <row r="84" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A84" s="116">
+      <c r="A84" s="95">
         <v>74</v>
       </c>
-      <c r="B84" s="115" t="s">
+      <c r="B84" s="94" t="s">
         <v>420</v>
       </c>
       <c r="C84" s="32" t="s">
@@ -7960,10 +7964,10 @@
       <c r="Z84" s="15"/>
     </row>
     <row r="85" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A85" s="116">
+      <c r="A85" s="95">
         <v>75</v>
       </c>
-      <c r="B85" s="115" t="s">
+      <c r="B85" s="94" t="s">
         <v>421</v>
       </c>
       <c r="C85" s="32" t="s">
@@ -8024,10 +8028,10 @@
       <c r="Z85" s="15"/>
     </row>
     <row r="86" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="116">
+      <c r="A86" s="95">
         <v>76</v>
       </c>
-      <c r="B86" s="115" t="s">
+      <c r="B86" s="94" t="s">
         <v>422</v>
       </c>
       <c r="C86" s="32" t="s">
@@ -8088,10 +8092,10 @@
       <c r="Z86" s="15"/>
     </row>
     <row r="87" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="116">
+      <c r="A87" s="95">
         <v>77</v>
       </c>
-      <c r="B87" s="115" t="s">
+      <c r="B87" s="94" t="s">
         <v>458</v>
       </c>
       <c r="C87" s="32" t="s">
@@ -8152,10 +8156,10 @@
       <c r="Z87" s="15"/>
     </row>
     <row r="88" spans="1:26" s="19" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="116">
+      <c r="A88" s="95">
         <v>78</v>
       </c>
-      <c r="B88" s="115" t="s">
+      <c r="B88" s="94" t="s">
         <v>423</v>
       </c>
       <c r="C88" s="32" t="s">
@@ -8216,10 +8220,10 @@
       <c r="Z88" s="38"/>
     </row>
     <row r="89" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="116">
+      <c r="A89" s="95">
         <v>79</v>
       </c>
-      <c r="B89" s="117" t="s">
+      <c r="B89" s="96" t="s">
         <v>424</v>
       </c>
       <c r="C89" s="17" t="s">
@@ -8280,10 +8284,10 @@
       <c r="Z89" s="15"/>
     </row>
     <row r="90" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="116">
+      <c r="A90" s="95">
         <v>80</v>
       </c>
-      <c r="B90" s="117" t="s">
+      <c r="B90" s="96" t="s">
         <v>425</v>
       </c>
       <c r="C90" s="17" t="s">
@@ -8344,10 +8348,10 @@
       <c r="Z90" s="15"/>
     </row>
     <row r="91" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="116">
+      <c r="A91" s="95">
         <v>81</v>
       </c>
-      <c r="B91" s="117" t="s">
+      <c r="B91" s="96" t="s">
         <v>457</v>
       </c>
       <c r="C91" s="17" t="s">
@@ -8410,6 +8414,11 @@
   </sheetData>
   <autoFilter ref="A8:U85" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="12">
+    <mergeCell ref="A10:U10"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="A60:U60"/>
+    <mergeCell ref="H6:T6"/>
     <mergeCell ref="A4:U4"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
@@ -8417,11 +8426,6 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="G6:G7"/>
-    <mergeCell ref="A10:U10"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="A60:U60"/>
-    <mergeCell ref="H6:T6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
@@ -8532,29 +8536,29 @@
       <c r="W3" s="46"/>
     </row>
     <row r="4" spans="1:23" s="47" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="104"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="104"/>
-      <c r="N4" s="104"/>
-      <c r="O4" s="104"/>
-      <c r="P4" s="104"/>
-      <c r="Q4" s="104"/>
-      <c r="R4" s="104"/>
-      <c r="S4" s="104"/>
-      <c r="T4" s="105"/>
-      <c r="U4" s="104"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="99"/>
+      <c r="N4" s="99"/>
+      <c r="O4" s="99"/>
+      <c r="P4" s="99"/>
+      <c r="Q4" s="99"/>
+      <c r="R4" s="99"/>
+      <c r="S4" s="99"/>
+      <c r="T4" s="100"/>
+      <c r="U4" s="99"/>
       <c r="V4" s="46"/>
       <c r="W4" s="46"/>
     </row>
@@ -8584,55 +8588,55 @@
       <c r="W5" s="46"/>
     </row>
     <row r="6" spans="1:23" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="110" t="s">
+      <c r="A6" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="108" t="s">
+      <c r="C6" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="110" t="s">
+      <c r="D6" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="110" t="s">
+      <c r="E6" s="114" t="s">
         <v>185</v>
       </c>
-      <c r="F6" s="108" t="s">
+      <c r="F6" s="112" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="96" t="s">
+      <c r="G6" s="101" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="100" t="s">
+      <c r="H6" s="108" t="s">
         <v>176</v>
       </c>
-      <c r="I6" s="101"/>
-      <c r="J6" s="101"/>
-      <c r="K6" s="101"/>
-      <c r="L6" s="101"/>
-      <c r="M6" s="101"/>
-      <c r="N6" s="101"/>
-      <c r="O6" s="101"/>
-      <c r="P6" s="101"/>
-      <c r="Q6" s="101"/>
-      <c r="R6" s="101"/>
-      <c r="S6" s="101"/>
-      <c r="T6" s="102"/>
-      <c r="U6" s="108" t="s">
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="109"/>
+      <c r="M6" s="109"/>
+      <c r="N6" s="109"/>
+      <c r="O6" s="109"/>
+      <c r="P6" s="109"/>
+      <c r="Q6" s="109"/>
+      <c r="R6" s="109"/>
+      <c r="S6" s="109"/>
+      <c r="T6" s="110"/>
+      <c r="U6" s="112" t="s">
         <v>7</v>
       </c>
       <c r="V6" s="48"/>
     </row>
     <row r="7" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="109"/>
-      <c r="B7" s="111"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="113"/>
-      <c r="G7" s="114"/>
+      <c r="A7" s="113"/>
+      <c r="B7" s="115"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="115"/>
+      <c r="E7" s="115"/>
+      <c r="F7" s="117"/>
+      <c r="G7" s="118"/>
       <c r="H7" s="20" t="s">
         <v>8</v>
       </c>
@@ -8672,7 +8676,7 @@
       <c r="T7" s="20" t="s">
         <v>614</v>
       </c>
-      <c r="U7" s="109"/>
+      <c r="U7" s="113"/>
       <c r="V7" s="48"/>
     </row>
     <row r="8" spans="1:23" s="47" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -8759,29 +8763,29 @@
       <c r="U9" s="53"/>
     </row>
     <row r="10" spans="1:23" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="107"/>
-      <c r="C10" s="107"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="107"/>
-      <c r="F10" s="107"/>
-      <c r="G10" s="107"/>
-      <c r="H10" s="107"/>
-      <c r="I10" s="107"/>
-      <c r="J10" s="107"/>
-      <c r="K10" s="107"/>
-      <c r="L10" s="107"/>
-      <c r="M10" s="107"/>
-      <c r="N10" s="107"/>
-      <c r="O10" s="107"/>
-      <c r="P10" s="107"/>
-      <c r="Q10" s="107"/>
-      <c r="R10" s="107"/>
-      <c r="S10" s="107"/>
-      <c r="T10" s="107"/>
-      <c r="U10" s="107"/>
+      <c r="B10" s="111"/>
+      <c r="C10" s="111"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="111"/>
+      <c r="G10" s="111"/>
+      <c r="H10" s="111"/>
+      <c r="I10" s="111"/>
+      <c r="J10" s="111"/>
+      <c r="K10" s="111"/>
+      <c r="L10" s="111"/>
+      <c r="M10" s="111"/>
+      <c r="N10" s="111"/>
+      <c r="O10" s="111"/>
+      <c r="P10" s="111"/>
+      <c r="Q10" s="111"/>
+      <c r="R10" s="111"/>
+      <c r="S10" s="111"/>
+      <c r="T10" s="111"/>
+      <c r="U10" s="111"/>
       <c r="V10" s="66"/>
     </row>
     <row r="11" spans="1:23" s="55" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.25">
@@ -10414,29 +10418,29 @@
       <c r="U37" s="53"/>
     </row>
     <row r="38" spans="1:22" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="94" t="s">
+      <c r="A38" s="103" t="s">
         <v>183</v>
       </c>
-      <c r="B38" s="107"/>
-      <c r="C38" s="107"/>
-      <c r="D38" s="107"/>
-      <c r="E38" s="107"/>
-      <c r="F38" s="107"/>
-      <c r="G38" s="107"/>
-      <c r="H38" s="107"/>
-      <c r="I38" s="107"/>
-      <c r="J38" s="107"/>
-      <c r="K38" s="107"/>
-      <c r="L38" s="107"/>
-      <c r="M38" s="107"/>
-      <c r="N38" s="107"/>
-      <c r="O38" s="107"/>
-      <c r="P38" s="107"/>
-      <c r="Q38" s="107"/>
-      <c r="R38" s="107"/>
-      <c r="S38" s="107"/>
-      <c r="T38" s="107"/>
-      <c r="U38" s="107"/>
+      <c r="B38" s="111"/>
+      <c r="C38" s="111"/>
+      <c r="D38" s="111"/>
+      <c r="E38" s="111"/>
+      <c r="F38" s="111"/>
+      <c r="G38" s="111"/>
+      <c r="H38" s="111"/>
+      <c r="I38" s="111"/>
+      <c r="J38" s="111"/>
+      <c r="K38" s="111"/>
+      <c r="L38" s="111"/>
+      <c r="M38" s="111"/>
+      <c r="N38" s="111"/>
+      <c r="O38" s="111"/>
+      <c r="P38" s="111"/>
+      <c r="Q38" s="111"/>
+      <c r="R38" s="111"/>
+      <c r="S38" s="111"/>
+      <c r="T38" s="111"/>
+      <c r="U38" s="111"/>
       <c r="V38" s="66"/>
     </row>
     <row r="39" spans="1:22" s="93" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>